<commit_message>
refactor: Clean input csv from empty lines
</commit_message>
<xml_diff>
--- a/inputData/Wikipedia_ICU.xlsx
+++ b/inputData/Wikipedia_ICU.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leopoldwalther/Documents/5_Projects/3_PythonProjects/AnalysisCovid19/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leopoldwalther/Documents/5_Projects/3_PythonProjects/AnalysisCovid19/inputData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6980F9D-49EC-284B-98E5-2B0BCAF48C9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB3C4D6-8CC8-0049-BE7C-712419C7E3A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{A8D48060-7358-6347-BA6B-34E7DC07248D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{A8D48060-7358-6347-BA6B-34E7DC07248D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -548,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F16B6C-72B2-8A40-8190-CC6438443D1A}">
-  <dimension ref="A2:F48"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -560,794 +560,785 @@
     <col min="5" max="5" width="28.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" t="s">
-        <v>53</v>
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>13.05</v>
+      </c>
+      <c r="D2">
+        <v>75.5</v>
+      </c>
+      <c r="E2">
+        <v>7.3</v>
+      </c>
+      <c r="F2" s="1">
+        <v>32586</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>13.05</v>
-      </c>
-      <c r="D3">
-        <v>75.5</v>
+        <v>12.27</v>
       </c>
       <c r="E3">
-        <v>7.3</v>
+        <v>10.6</v>
       </c>
       <c r="F3" s="1">
-        <v>32586</v>
+        <v>9795</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>12.27</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="E4">
-        <v>10.6</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="F4" s="1">
-        <v>9795</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5">
-        <v>8.0500000000000007</v>
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>79.8</v>
       </c>
       <c r="E5">
-        <v>8.3000000000000007</v>
+        <v>33.9</v>
       </c>
       <c r="F5" s="1">
         <v>40000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>7.37</v>
       </c>
       <c r="D6">
-        <v>79.8</v>
+        <v>73.8</v>
       </c>
       <c r="E6">
-        <v>33.9</v>
+        <v>21.8</v>
       </c>
       <c r="F6" s="1">
-        <v>40000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>7.37</v>
+        <v>7.02</v>
       </c>
       <c r="D7">
-        <v>73.8</v>
+        <v>65.5</v>
       </c>
       <c r="E7">
-        <v>21.8</v>
+        <v>13.8</v>
       </c>
       <c r="F7" s="1">
-        <v>2500</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8">
-        <v>7.02</v>
+        <v>6.63</v>
       </c>
       <c r="D8">
-        <v>65.5</v>
+        <v>70.099999999999994</v>
       </c>
       <c r="E8">
-        <v>13.8</v>
+        <v>11.6</v>
       </c>
       <c r="F8" s="1">
-        <v>2560</v>
+        <v>3529</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
       </c>
       <c r="C9">
-        <v>6.63</v>
-      </c>
-      <c r="D9">
-        <v>70.099999999999994</v>
+        <v>6.62</v>
       </c>
       <c r="E9">
-        <v>11.6</v>
+        <v>6.9</v>
       </c>
       <c r="F9" s="1">
-        <v>3529</v>
+        <v>10100</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="C10">
-        <v>6.62</v>
+        <v>6.56</v>
+      </c>
+      <c r="D10">
+        <v>73.2</v>
       </c>
       <c r="E10">
-        <v>6.9</v>
+        <v>15.5</v>
       </c>
       <c r="F10" s="1">
-        <v>10100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
       <c r="C11">
-        <v>6.56</v>
+        <v>5.98</v>
       </c>
       <c r="D11">
-        <v>73.2</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="E11">
-        <v>15.5</v>
+        <v>11.6</v>
       </c>
       <c r="F11" s="1">
-        <v>1000</v>
+        <v>7007</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
       </c>
       <c r="C12">
-        <v>5.98</v>
+        <v>5.82</v>
       </c>
       <c r="D12">
-        <v>75.599999999999994</v>
+        <v>67.8</v>
       </c>
       <c r="E12">
-        <v>11.6</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="F12" s="1">
-        <v>7007</v>
+        <v>600</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
       </c>
       <c r="C13">
-        <v>5.82</v>
+        <v>5.76</v>
       </c>
       <c r="D13">
-        <v>67.8</v>
+        <v>81.8</v>
       </c>
       <c r="E13">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="F13" s="1">
-        <v>600</v>
-      </c>
+        <v>15.9</v>
+      </c>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
       </c>
       <c r="C14">
-        <v>5.76</v>
+        <v>5.57</v>
       </c>
       <c r="D14">
-        <v>81.8</v>
+        <v>71.099999999999994</v>
       </c>
       <c r="E14">
-        <v>15.9</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>5.57</v>
-      </c>
-      <c r="D15">
-        <v>71.099999999999994</v>
+        <v>5.4</v>
       </c>
       <c r="E15">
-        <v>9.6999999999999993</v>
+        <v>7.1</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>5.4</v>
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="D16">
+        <v>70.400000000000006</v>
       </c>
       <c r="E16">
-        <v>7.1</v>
+        <v>14.6</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
       </c>
       <c r="C17">
-        <v>4.6900000000000004</v>
+        <v>4.66</v>
       </c>
       <c r="D17">
-        <v>70.400000000000006</v>
+        <v>70.7</v>
       </c>
       <c r="E17">
-        <v>14.6</v>
+        <v>24.8</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>4</v>
       </c>
       <c r="C18">
-        <v>4.66</v>
+        <v>4.53</v>
       </c>
       <c r="D18">
-        <v>70.7</v>
+        <v>82</v>
       </c>
       <c r="E18">
-        <v>24.8</v>
+        <v>11</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>4</v>
       </c>
       <c r="C19">
-        <v>4.53</v>
+        <v>4.5</v>
       </c>
       <c r="D19">
-        <v>82</v>
+        <v>69.5</v>
       </c>
       <c r="E19">
-        <v>11</v>
+        <v>6.4</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>4.5</v>
-      </c>
-      <c r="D20">
-        <v>69.5</v>
+        <v>4.34</v>
       </c>
       <c r="E20">
-        <v>6.4</v>
+        <v>3.6</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C21">
-        <v>4.34</v>
+        <v>4.21</v>
+      </c>
+      <c r="D21">
+        <v>61.6</v>
       </c>
       <c r="E21">
-        <v>3.6</v>
+        <v>6</v>
       </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C22">
-        <v>4.21</v>
-      </c>
-      <c r="D22">
-        <v>61.6</v>
+        <v>3.84</v>
       </c>
       <c r="E22">
-        <v>6</v>
-      </c>
-      <c r="F22" s="1"/>
+        <v>9.1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1314</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C23">
-        <v>3.84</v>
+        <v>3.6</v>
+      </c>
+      <c r="D23">
+        <v>80.7</v>
       </c>
       <c r="E23">
-        <v>9.1</v>
+        <v>8</v>
       </c>
       <c r="F23" s="1">
-        <v>1314</v>
+        <v>800</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
       </c>
       <c r="C24">
-        <v>3.6</v>
+        <v>3.39</v>
       </c>
       <c r="D24">
-        <v>80.7</v>
+        <v>66.8</v>
       </c>
       <c r="E24">
-        <v>8</v>
+        <v>4.2</v>
       </c>
       <c r="F24" s="1">
-        <v>800</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
         <v>4</v>
       </c>
       <c r="C25">
-        <v>3.39</v>
+        <v>3.32</v>
       </c>
       <c r="D25">
-        <v>66.8</v>
+        <v>65.400000000000006</v>
       </c>
       <c r="E25">
-        <v>4.2</v>
-      </c>
-      <c r="F25" s="1">
-        <v>1400</v>
-      </c>
+        <v>6.4</v>
+      </c>
+      <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
       </c>
       <c r="C26">
-        <v>3.32</v>
-      </c>
-      <c r="D26">
-        <v>65.400000000000006</v>
+        <v>3.28</v>
       </c>
       <c r="E26">
-        <v>6.4</v>
+        <v>6.1</v>
       </c>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
       </c>
       <c r="C27">
-        <v>3.28</v>
+        <v>3.18</v>
+      </c>
+      <c r="D27">
+        <v>78.900000000000006</v>
       </c>
       <c r="E27">
-        <v>6.1</v>
-      </c>
-      <c r="F27" s="1"/>
+        <v>12.5</v>
+      </c>
+      <c r="F27" s="1">
+        <v>5324</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
       </c>
       <c r="C28">
-        <v>3.18</v>
-      </c>
-      <c r="D28">
-        <v>78.900000000000006</v>
+        <v>3.06</v>
       </c>
       <c r="E28">
-        <v>12.5</v>
-      </c>
-      <c r="F28" s="1">
-        <v>5324</v>
-      </c>
+        <v>9.1</v>
+      </c>
+      <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C29">
-        <v>3.06</v>
-      </c>
-      <c r="E29">
-        <v>9.1</v>
+        <v>3.02</v>
+      </c>
+      <c r="D29">
+        <v>93.3</v>
       </c>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C30">
-        <v>3.02</v>
+        <v>2.97</v>
       </c>
       <c r="D30">
-        <v>93.3</v>
+        <v>75.3</v>
+      </c>
+      <c r="E30">
+        <v>9.6999999999999993</v>
       </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
         <v>4</v>
       </c>
       <c r="C31">
-        <v>2.97</v>
+        <v>2.96</v>
       </c>
       <c r="D31">
-        <v>75.3</v>
+        <v>94.9</v>
       </c>
       <c r="E31">
-        <v>9.6999999999999993</v>
+        <v>6.5</v>
       </c>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
         <v>4</v>
       </c>
       <c r="C32">
-        <v>2.96</v>
+        <v>2.81</v>
       </c>
       <c r="D32">
-        <v>94.9</v>
+        <v>68</v>
       </c>
       <c r="E32">
-        <v>6.5</v>
-      </c>
-      <c r="F32" s="1"/>
+        <v>46.5</v>
+      </c>
+      <c r="F32" s="1">
+        <v>17000</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="C33">
-        <v>2.81</v>
+        <v>2.77</v>
       </c>
       <c r="D33">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E33">
-        <v>46.5</v>
+        <v>29.4</v>
       </c>
       <c r="F33" s="1">
-        <v>17000</v>
+        <v>68000</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C34">
-        <v>2.77</v>
-      </c>
-      <c r="D34">
-        <v>64</v>
+        <v>2.71</v>
       </c>
       <c r="E34">
-        <v>29.4</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="F34" s="1">
-        <v>68000</v>
+        <v>334</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C35">
-        <v>2.71</v>
+        <v>2.61</v>
       </c>
       <c r="E35">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="F35" s="1">
-        <v>334</v>
-      </c>
+        <v>6.7</v>
+      </c>
+      <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
         <v>4</v>
       </c>
       <c r="C36">
-        <v>2.61</v>
+        <v>2.54</v>
+      </c>
+      <c r="D36">
+        <v>84.3</v>
       </c>
       <c r="E36">
-        <v>6.7</v>
-      </c>
-      <c r="F36" s="1"/>
+        <v>6.6</v>
+      </c>
+      <c r="F36" s="1">
+        <v>8175</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="C37">
-        <v>2.54</v>
+        <v>2.52</v>
       </c>
       <c r="D37">
-        <v>84.3</v>
+        <v>91.6</v>
       </c>
       <c r="E37">
-        <v>6.6</v>
-      </c>
-      <c r="F37" s="1">
-        <v>8175</v>
-      </c>
+        <v>13.5</v>
+      </c>
+      <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C38">
-        <v>2.52</v>
-      </c>
-      <c r="D38">
-        <v>91.6</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="E38">
-        <v>13.5</v>
-      </c>
-      <c r="F38" s="1"/>
+        <v>5.8</v>
+      </c>
+      <c r="F38" s="1">
+        <v>570</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="C39">
-        <v>2.2200000000000002</v>
-      </c>
-      <c r="E39">
-        <v>5.8</v>
-      </c>
-      <c r="F39" s="1">
-        <v>570</v>
-      </c>
+        <v>2.11</v>
+      </c>
+      <c r="D39">
+        <v>79.099999999999994</v>
+      </c>
+      <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
         <v>41</v>
       </c>
       <c r="C40">
-        <v>2.11</v>
-      </c>
-      <c r="D40">
-        <v>79.099999999999994</v>
+        <v>1.7</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="C41">
-        <v>1.7</v>
-      </c>
-      <c r="F41" s="1"/>
+        <v>0.53</v>
+      </c>
+      <c r="F41" s="1">
+        <v>40000</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="C42">
-        <v>0.53</v>
+        <v>1.38</v>
+      </c>
+      <c r="D42">
+        <v>74</v>
+      </c>
+      <c r="E42" t="s">
+        <v>54</v>
       </c>
       <c r="F42" s="1">
-        <v>40000</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C43">
-        <v>1.38</v>
-      </c>
-      <c r="D43">
-        <v>74</v>
-      </c>
-      <c r="E43" t="s">
-        <v>54</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="F43" s="1">
-        <v>2050</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C44">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="F44" s="1">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>46</v>
-      </c>
-      <c r="B45" t="s">
-        <v>1</v>
-      </c>
-      <c r="C45">
         <v>0.87</v>
       </c>
-      <c r="E45">
+      <c r="E44">
         <v>0.72</v>
       </c>
-      <c r="F45" s="1"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F48" s="1"/>
+      <c r="F44" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
refactor: Change column name in input xlsx and csv
</commit_message>
<xml_diff>
--- a/inputData/Wikipedia_ICU.xlsx
+++ b/inputData/Wikipedia_ICU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leopoldwalther/Documents/5_Projects/3_PythonProjects/AnalysisCovid19/inputData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB3C4D6-8CC8-0049-BE7C-712419C7E3A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B19B25-5AB4-9B49-B21D-6D8084AE341F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{A8D48060-7358-6347-BA6B-34E7DC07248D}"/>
   </bookViews>
@@ -180,9 +180,6 @@
     <t>hospital_beds_per_1000_people</t>
   </si>
   <si>
-    <t>country</t>
-  </si>
-  <si>
     <t>continent</t>
   </si>
   <si>
@@ -196,6 +193,9 @@
   </si>
   <si>
     <t> 1.2</t>
+  </si>
+  <si>
+    <t>countryname</t>
   </si>
 </sst>
 </file>
@@ -550,9 +550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F16B6C-72B2-8A40-8190-CC6438443D1A}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -562,22 +560,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
         <v>49</v>
-      </c>
-      <c r="B1" t="s">
-        <v>50</v>
       </c>
       <c r="C1" t="s">
         <v>48</v>
       </c>
       <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
         <v>51</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>52</v>
-      </c>
-      <c r="F1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1305,7 +1303,7 @@
         <v>74</v>
       </c>
       <c r="E42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F42" s="1">
         <v>2050</v>

</xml_diff>

<commit_message>
feat: Finalize clean up of dataframes and storage
</commit_message>
<xml_diff>
--- a/inputData/Wikipedia_ICU.xlsx
+++ b/inputData/Wikipedia_ICU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leopoldwalther/Documents/5_Projects/3_PythonProjects/AnalysisCovid19/inputData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B19B25-5AB4-9B49-B21D-6D8084AE341F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03041402-9713-2E46-B67D-F3B55C2E91BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{A8D48060-7358-6347-BA6B-34E7DC07248D}"/>
   </bookViews>
@@ -233,7 +233,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,9 +548,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F16B6C-72B2-8A40-8190-CC6438443D1A}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:P1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -585,13 +587,13 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>13.05</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>75.5</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>7.3</v>
       </c>
       <c r="F2" s="1">
@@ -605,10 +607,11 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>12.27</v>
       </c>
-      <c r="E3">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1">
         <v>10.6</v>
       </c>
       <c r="F3" s="1">
@@ -622,10 +625,11 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>8.0500000000000007</v>
       </c>
-      <c r="E4">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1">
         <v>8.3000000000000007</v>
       </c>
       <c r="F4" s="1">
@@ -639,13 +643,13 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>8</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>79.8</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>33.9</v>
       </c>
       <c r="F5" s="1">
@@ -659,13 +663,13 @@
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>7.37</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>73.8</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>21.8</v>
       </c>
       <c r="F6" s="1">
@@ -679,13 +683,13 @@
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>7.02</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>65.5</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>13.8</v>
       </c>
       <c r="F7" s="1">
@@ -699,13 +703,13 @@
       <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>6.63</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>70.099999999999994</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>11.6</v>
       </c>
       <c r="F8" s="1">
@@ -719,10 +723,11 @@
       <c r="B9" t="s">
         <v>4</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>6.62</v>
       </c>
-      <c r="E9">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1">
         <v>6.9</v>
       </c>
       <c r="F9" s="1">
@@ -736,13 +741,13 @@
       <c r="B10" t="s">
         <v>4</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>6.56</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>73.2</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>15.5</v>
       </c>
       <c r="F10" s="1">
@@ -756,13 +761,13 @@
       <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>5.98</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>75.599999999999994</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>11.6</v>
       </c>
       <c r="F11" s="1">
@@ -776,13 +781,13 @@
       <c r="B12" t="s">
         <v>4</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>5.82</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>67.8</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>9.1999999999999993</v>
       </c>
       <c r="F12" s="1">
@@ -796,13 +801,13 @@
       <c r="B13" t="s">
         <v>4</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>5.76</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>81.8</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>15.9</v>
       </c>
       <c r="F13" s="1"/>
@@ -814,13 +819,13 @@
       <c r="B14" t="s">
         <v>4</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>5.57</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>71.099999999999994</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>9.6999999999999993</v>
       </c>
       <c r="F14" s="1"/>
@@ -832,10 +837,11 @@
       <c r="B15" t="s">
         <v>1</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>5.4</v>
       </c>
-      <c r="E15">
+      <c r="D15" s="1"/>
+      <c r="E15" s="1">
         <v>7.1</v>
       </c>
       <c r="F15" s="1"/>
@@ -847,13 +853,13 @@
       <c r="B16" t="s">
         <v>4</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>4.6900000000000004</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>70.400000000000006</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>14.6</v>
       </c>
       <c r="F16" s="1"/>
@@ -865,13 +871,13 @@
       <c r="B17" t="s">
         <v>4</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>4.66</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>70.7</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <v>24.8</v>
       </c>
       <c r="F17" s="1"/>
@@ -883,13 +889,13 @@
       <c r="B18" t="s">
         <v>4</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>4.53</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>82</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>11</v>
       </c>
       <c r="F18" s="1"/>
@@ -901,13 +907,13 @@
       <c r="B19" t="s">
         <v>4</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>4.5</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>69.5</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <v>6.4</v>
       </c>
       <c r="F19" s="1"/>
@@ -919,10 +925,11 @@
       <c r="B20" t="s">
         <v>1</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>4.34</v>
       </c>
-      <c r="E20">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1">
         <v>3.6</v>
       </c>
       <c r="F20" s="1"/>
@@ -934,13 +941,13 @@
       <c r="B21" t="s">
         <v>4</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>4.21</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>61.6</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <v>6</v>
       </c>
       <c r="F21" s="1"/>
@@ -952,10 +959,11 @@
       <c r="B22" t="s">
         <v>23</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>3.84</v>
       </c>
-      <c r="E22">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1">
         <v>9.1</v>
       </c>
       <c r="F22" s="1">
@@ -969,13 +977,13 @@
       <c r="B23" t="s">
         <v>4</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>3.6</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>80.7</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="1">
         <v>8</v>
       </c>
       <c r="F23" s="1">
@@ -989,13 +997,13 @@
       <c r="B24" t="s">
         <v>4</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>3.39</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>66.8</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="1">
         <v>4.2</v>
       </c>
       <c r="F24" s="1">
@@ -1009,13 +1017,13 @@
       <c r="B25" t="s">
         <v>4</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>3.32</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>65.400000000000006</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="1">
         <v>6.4</v>
       </c>
       <c r="F25" s="1"/>
@@ -1027,10 +1035,11 @@
       <c r="B26" t="s">
         <v>4</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>3.28</v>
       </c>
-      <c r="E26">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1">
         <v>6.1</v>
       </c>
       <c r="F26" s="1"/>
@@ -1042,13 +1051,13 @@
       <c r="B27" t="s">
         <v>4</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>3.18</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>78.900000000000006</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="1">
         <v>12.5</v>
       </c>
       <c r="F27" s="1">
@@ -1062,10 +1071,11 @@
       <c r="B28" t="s">
         <v>4</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>3.06</v>
       </c>
-      <c r="E28">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1">
         <v>9.1</v>
       </c>
       <c r="F28" s="1"/>
@@ -1077,12 +1087,13 @@
       <c r="B29" t="s">
         <v>1</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>3.02</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>93.3</v>
       </c>
+      <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1092,13 +1103,13 @@
       <c r="B30" t="s">
         <v>4</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>2.97</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
         <v>75.3</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="1">
         <v>9.6999999999999993</v>
       </c>
       <c r="F30" s="1"/>
@@ -1110,13 +1121,13 @@
       <c r="B31" t="s">
         <v>4</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <v>2.96</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>94.9</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="1">
         <v>6.5</v>
       </c>
       <c r="F31" s="1"/>
@@ -1128,13 +1139,13 @@
       <c r="B32" t="s">
         <v>4</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
         <v>2.81</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
         <v>68</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="1">
         <v>46.5</v>
       </c>
       <c r="F32" s="1">
@@ -1148,13 +1159,13 @@
       <c r="B33" t="s">
         <v>35</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <v>2.77</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>64</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="1">
         <v>29.4</v>
       </c>
       <c r="F33" s="1">
@@ -1168,10 +1179,11 @@
       <c r="B34" t="s">
         <v>23</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
         <v>2.71</v>
       </c>
-      <c r="E34">
+      <c r="D34" s="1"/>
+      <c r="E34" s="1">
         <v>4.5999999999999996</v>
       </c>
       <c r="F34" s="1">
@@ -1185,10 +1197,11 @@
       <c r="B35" t="s">
         <v>4</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <v>2.61</v>
       </c>
-      <c r="E35">
+      <c r="D35" s="1"/>
+      <c r="E35" s="1">
         <v>6.7</v>
       </c>
       <c r="F35" s="1"/>
@@ -1200,13 +1213,13 @@
       <c r="B36" t="s">
         <v>4</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
         <v>2.54</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="1">
         <v>84.3</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="1">
         <v>6.6</v>
       </c>
       <c r="F36" s="1">
@@ -1220,13 +1233,13 @@
       <c r="B37" t="s">
         <v>35</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <v>2.52</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
         <v>91.6</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="1">
         <v>13.5</v>
       </c>
       <c r="F37" s="1"/>
@@ -1238,10 +1251,11 @@
       <c r="B38" t="s">
         <v>4</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <v>2.2200000000000002</v>
       </c>
-      <c r="E38">
+      <c r="D38" s="1"/>
+      <c r="E38" s="1">
         <v>5.8</v>
       </c>
       <c r="F38" s="1">
@@ -1255,12 +1269,13 @@
       <c r="B39" t="s">
         <v>41</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="1">
         <v>2.11</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="1">
         <v>79.099999999999994</v>
       </c>
+      <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -1270,9 +1285,11 @@
       <c r="B40" t="s">
         <v>41</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="1">
         <v>1.7</v>
       </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1282,9 +1299,11 @@
       <c r="B41" t="s">
         <v>1</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="1">
         <v>0.53</v>
       </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
       <c r="F41" s="1">
         <v>40000</v>
       </c>
@@ -1296,13 +1315,13 @@
       <c r="B42" t="s">
         <v>35</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="1">
         <v>1.38</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
         <v>74</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="1" t="s">
         <v>53</v>
       </c>
       <c r="F42" s="1">
@@ -1316,9 +1335,11 @@
       <c r="B43" t="s">
         <v>4</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="1">
         <v>8.8000000000000007</v>
       </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
       <c r="F43" s="1">
         <v>3600</v>
       </c>
@@ -1330,13 +1351,20 @@
       <c r="B44" t="s">
         <v>1</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="1">
         <v>0.87</v>
       </c>
-      <c r="E44">
+      <c r="D44" s="1"/>
+      <c r="E44" s="1">
         <v>0.72</v>
       </c>
       <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>